<commit_message>
Notas AVs Wyden UniRuy 23062025
</commit_message>
<xml_diff>
--- a/05 Others/Linguagem C AV Media Final Wyden Uniruy 2025_1.xlsx
+++ b/05 Others/Linguagem C AV Media Final Wyden Uniruy 2025_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heleno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE02DD6F-3678-41CC-B8F2-E8D181CC9F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B5FADD-287B-4DD0-B1BB-63BB59BEA059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00CE2D0E-0A12-41EE-A73B-9B255E59C8BB}"/>
   </bookViews>
@@ -260,7 +260,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +285,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -527,7 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -554,25 +560,31 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -911,7 +923,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -920,8 +932,8 @@
     <col min="2" max="2" width="84.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="98.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="6"/>
@@ -943,37 +955,41 @@
       <c r="E1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>50</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+      <c r="A2" s="13">
         <v>3001</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="17">
-        <v>0.8</v>
-      </c>
-      <c r="D2" s="17">
-        <v>0.7</v>
-      </c>
-      <c r="E2" s="22">
+      <c r="C2" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="E2" s="16">
         <v>0</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19">
-        <f>SUM(C2:G2)</f>
-        <v>1.5</v>
+      <c r="F2" s="19">
+        <v>3.8</v>
+      </c>
+      <c r="G2" s="20">
+        <v>3.6</v>
+      </c>
+      <c r="H2" s="21">
+        <f t="shared" ref="H2:H42" si="0">SUM(C2:G2)</f>
+        <v>8.9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -992,11 +1008,15 @@
       <c r="E3" s="10">
         <v>2</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="12">
-        <f t="shared" ref="H3:H42" si="0">SUM(C3:G3)</f>
-        <v>3.3</v>
+      <c r="F3" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="G3" s="23">
+        <v>2</v>
+      </c>
+      <c r="H3" s="24">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
       </c>
       <c r="I3" s="8"/>
     </row>
@@ -1004,7 +1024,7 @@
       <c r="A4" s="7">
         <v>3001</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="10">
@@ -1013,35 +1033,43 @@
       <c r="D4" s="10">
         <v>0.6</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="17">
         <v>0</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="12">
-        <f t="shared" si="0"/>
-        <v>1.4</v>
+      <c r="F4" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="G4" s="23">
+        <v>3.6</v>
+      </c>
+      <c r="H4" s="24">
+        <f t="shared" si="0"/>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3001</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="15">
         <v>0</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="12">
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1062,11 +1090,15 @@
       <c r="E6" s="10">
         <v>2</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="12">
-        <f t="shared" si="0"/>
-        <v>3.3</v>
+      <c r="F6" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="G6" s="23">
+        <v>3.6</v>
+      </c>
+      <c r="H6" s="24">
+        <f t="shared" si="0"/>
+        <v>10.4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1085,11 +1117,15 @@
       <c r="E7" s="10">
         <v>2</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="12">
-        <f t="shared" si="0"/>
-        <v>3.4</v>
+      <c r="F7" s="22">
+        <v>2</v>
+      </c>
+      <c r="G7" s="23">
+        <v>2</v>
+      </c>
+      <c r="H7" s="24">
+        <f t="shared" si="0"/>
+        <v>7.4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1108,11 +1144,15 @@
       <c r="E8" s="10">
         <v>2</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="12">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
+      <c r="F8" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="G8" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="H8" s="24">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>54</v>
@@ -1134,11 +1174,15 @@
       <c r="E9" s="10">
         <v>2</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="12">
-        <f t="shared" si="0"/>
-        <v>3.4</v>
+      <c r="F9" s="22">
+        <v>3.6</v>
+      </c>
+      <c r="G9" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="H9" s="24">
+        <f t="shared" si="0"/>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1157,11 +1201,15 @@
       <c r="E10" s="10">
         <v>2</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="12">
-        <f t="shared" si="0"/>
-        <v>3.1</v>
+      <c r="F10" s="22">
+        <v>2</v>
+      </c>
+      <c r="G10" s="23">
+        <v>2.8</v>
+      </c>
+      <c r="H10" s="24">
+        <f t="shared" si="0"/>
+        <v>7.8999999999999995</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>55</v>
@@ -1183,18 +1231,22 @@
       <c r="E11" s="10">
         <v>2</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="12">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
+      <c r="F11" s="22">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G11" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="H11" s="24">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>3001</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1203,14 +1255,18 @@
       <c r="D12" s="10">
         <v>0.3</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="17">
         <v>0</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="12">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
+      <c r="F12" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="23">
+        <v>2.4</v>
+      </c>
+      <c r="H12" s="28">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1229,11 +1285,15 @@
       <c r="E13" s="10">
         <v>2</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="12">
-        <f t="shared" si="0"/>
-        <v>3.4</v>
+      <c r="F13" s="22">
+        <v>4</v>
+      </c>
+      <c r="G13" s="23">
+        <v>1.6</v>
+      </c>
+      <c r="H13" s="24">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1252,11 +1312,15 @@
       <c r="E14" s="10">
         <v>2</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="12">
-        <f t="shared" si="0"/>
-        <v>3.1</v>
+      <c r="F14" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="G14" s="23">
+        <v>3.6</v>
+      </c>
+      <c r="H14" s="24">
+        <f t="shared" si="0"/>
+        <v>10.4</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1275,11 +1339,15 @@
       <c r="E15" s="10">
         <v>2</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="12">
-        <f t="shared" si="0"/>
+      <c r="F15" s="22">
+        <v>2</v>
+      </c>
+      <c r="G15" s="23">
         <v>3.2</v>
+      </c>
+      <c r="H15" s="24">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1298,11 +1366,15 @@
       <c r="E16" s="10">
         <v>2</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="12">
-        <f t="shared" si="0"/>
+      <c r="F16" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="G16" s="23">
         <v>2.8</v>
+      </c>
+      <c r="H16" s="24">
+        <f t="shared" si="0"/>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1321,11 +1393,15 @@
       <c r="E17" s="10">
         <v>2</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="12">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
+      <c r="F17" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="G17" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="H17" s="24">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>56</v>
@@ -1347,32 +1423,40 @@
       <c r="E18" s="10">
         <v>2</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="12">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
+      <c r="F18" s="22">
+        <v>3.4</v>
+      </c>
+      <c r="G18" s="23">
+        <v>1.6</v>
+      </c>
+      <c r="H18" s="24">
+        <f t="shared" si="0"/>
+        <v>7.7999999999999989</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>3001</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="15">
         <v>0.4</v>
       </c>
-      <c r="D19" s="21">
-        <v>0.7</v>
-      </c>
-      <c r="E19" s="21">
+      <c r="D19" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="E19" s="15">
         <v>0</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="12">
+      <c r="F19" s="15">
+        <v>0</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0</v>
+      </c>
+      <c r="H19" s="28">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
@@ -1393,11 +1477,15 @@
       <c r="E20" s="10">
         <v>2</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="12">
-        <f t="shared" si="0"/>
+      <c r="F20" s="22">
         <v>3.6</v>
+      </c>
+      <c r="G20" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="H20" s="24">
+        <f t="shared" si="0"/>
+        <v>10.4</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1416,18 +1504,22 @@
       <c r="E21" s="10">
         <v>2</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="12">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
+      <c r="F21" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="G21" s="23">
+        <v>3.6</v>
+      </c>
+      <c r="H21" s="24">
+        <f t="shared" si="0"/>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>3001</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="10">
@@ -1439,11 +1531,15 @@
       <c r="E22" s="10">
         <v>2</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="12">
-        <f t="shared" si="0"/>
-        <v>3.1</v>
+      <c r="F22" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="G22" s="23">
+        <v>3.6</v>
+      </c>
+      <c r="H22" s="24">
+        <f t="shared" si="0"/>
+        <v>10.199999999999999</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>59</v>
@@ -1465,11 +1561,15 @@
       <c r="E23" s="10">
         <v>2</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="12">
-        <f t="shared" si="0"/>
-        <v>2.9</v>
+      <c r="F23" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="G23" s="23">
+        <v>2</v>
+      </c>
+      <c r="H23" s="24">
+        <f t="shared" si="0"/>
+        <v>6.1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1485,16 +1585,20 @@
       <c r="D24" s="10">
         <v>0.8</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="17">
         <v>1.5</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="12">
-        <f t="shared" si="0"/>
-        <v>2.7</v>
-      </c>
-      <c r="I24" s="25" t="s">
+      <c r="F24" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="G24" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="H24" s="24">
+        <f t="shared" si="0"/>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="I24" s="18" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1514,11 +1618,15 @@
       <c r="E25" s="10">
         <v>2</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="12">
-        <f t="shared" si="0"/>
-        <v>3.3</v>
+      <c r="F25" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="G25" s="23">
+        <v>3.6</v>
+      </c>
+      <c r="H25" s="24">
+        <f t="shared" si="0"/>
+        <v>10.7</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>58</v>
@@ -1540,32 +1648,40 @@
       <c r="E26" s="10">
         <v>2</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="12">
-        <f t="shared" si="0"/>
-        <v>3.3</v>
+      <c r="F26" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="G26" s="23">
+        <v>2.8</v>
+      </c>
+      <c r="H26" s="24">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>3001</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="15">
         <v>0</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="12">
+      <c r="F27" s="15">
+        <v>0</v>
+      </c>
+      <c r="G27" s="15">
+        <v>0</v>
+      </c>
+      <c r="H27" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1574,21 +1690,25 @@
       <c r="A28" s="7">
         <v>3001</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="15">
         <v>0</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="12">
+      <c r="F28" s="15">
+        <v>0</v>
+      </c>
+      <c r="G28" s="15">
+        <v>0</v>
+      </c>
+      <c r="H28" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1609,18 +1729,22 @@
       <c r="E29" s="10">
         <v>2</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="12">
-        <f t="shared" si="0"/>
-        <v>3.4</v>
+      <c r="F29" s="22">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G29" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="H29" s="24">
+        <f t="shared" si="0"/>
+        <v>8.8999999999999986</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>3001</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="10">
@@ -1629,35 +1753,43 @@
       <c r="D30" s="10">
         <v>0.8</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="17">
         <v>0</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="12">
-        <f t="shared" si="0"/>
-        <v>1.3</v>
+      <c r="F30" s="22">
+        <v>3.4</v>
+      </c>
+      <c r="G30" s="23">
+        <v>2.4</v>
+      </c>
+      <c r="H30" s="24">
+        <f t="shared" si="0"/>
+        <v>7.1</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>3035</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="15">
         <v>0.2</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="15">
         <v>0</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="12">
+      <c r="F31" s="15">
+        <v>0</v>
+      </c>
+      <c r="G31" s="15">
+        <v>0</v>
+      </c>
+      <c r="H31" s="32">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
@@ -1678,11 +1810,15 @@
       <c r="E32" s="10">
         <v>2</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="12">
-        <f t="shared" si="0"/>
-        <v>3.1</v>
+      <c r="F32" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="G32" s="23">
+        <v>2.8</v>
+      </c>
+      <c r="H32" s="24">
+        <f t="shared" si="0"/>
+        <v>6.1</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>51</v>
@@ -1704,18 +1840,22 @@
       <c r="E33" s="10">
         <v>2</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="12">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
+      <c r="F33" s="22">
+        <v>2</v>
+      </c>
+      <c r="G33" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="H33" s="24">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>3035</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="17" t="s">
         <v>39</v>
       </c>
       <c r="C34" s="10">
@@ -1724,35 +1864,43 @@
       <c r="D34" s="10">
         <v>0.6</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="17">
         <v>0</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="12">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+      <c r="F34" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="G34" s="23">
+        <v>3.6</v>
+      </c>
+      <c r="H34" s="24">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>3035</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="15">
         <v>0</v>
       </c>
-      <c r="F35" s="21"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="12">
+      <c r="F35" s="15">
+        <v>0</v>
+      </c>
+      <c r="G35" s="15">
+        <v>0</v>
+      </c>
+      <c r="H35" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1773,11 +1921,15 @@
       <c r="E36" s="10">
         <v>2</v>
       </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="12">
-        <f t="shared" si="0"/>
-        <v>3.3</v>
+      <c r="F36" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="G36" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="H36" s="24">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1796,11 +1948,15 @@
       <c r="E37" s="10">
         <v>2</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="12">
-        <f t="shared" si="0"/>
-        <v>3.2</v>
+      <c r="F37" s="22">
+        <v>4</v>
+      </c>
+      <c r="G37" s="23">
+        <v>2.8</v>
+      </c>
+      <c r="H37" s="24">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>52</v>
@@ -1822,11 +1978,15 @@
       <c r="E38" s="10">
         <v>2</v>
       </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="12">
-        <f t="shared" si="0"/>
-        <v>3.3</v>
+      <c r="F38" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="G38" s="23">
+        <v>2</v>
+      </c>
+      <c r="H38" s="24">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1845,11 +2005,15 @@
       <c r="E39" s="10">
         <v>2</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="12">
-        <f t="shared" si="0"/>
+      <c r="F39" s="22">
+        <v>4</v>
+      </c>
+      <c r="G39" s="23">
         <v>3.2</v>
+      </c>
+      <c r="H39" s="24">
+        <f t="shared" si="0"/>
+        <v>10.4</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>53</v>
@@ -1859,7 +2023,7 @@
       <c r="A40" s="7">
         <v>3035</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="31" t="s">
         <v>45</v>
       </c>
       <c r="C40" s="10">
@@ -1871,11 +2035,15 @@
       <c r="E40" s="10">
         <v>2</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="12">
-        <f t="shared" si="0"/>
-        <v>2.9</v>
+      <c r="F40" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="G40" s="23">
+        <v>2</v>
+      </c>
+      <c r="H40" s="30">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1894,11 +2062,15 @@
       <c r="E41" s="10">
         <v>2</v>
       </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="12">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
+      <c r="F41" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="23">
+        <v>2.8</v>
+      </c>
+      <c r="H41" s="24">
+        <f t="shared" si="0"/>
+        <v>6.8</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1917,11 +2089,15 @@
       <c r="E42" s="11">
         <v>2</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="20">
-        <f t="shared" si="0"/>
-        <v>3.4</v>
+      <c r="F42" s="25">
+        <v>4</v>
+      </c>
+      <c r="G42" s="26">
+        <v>3.2</v>
+      </c>
+      <c r="H42" s="27">
+        <f t="shared" si="0"/>
+        <v>10.600000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>